<commit_message>
Actualiza múltiples plantillas de Excel y el historial de clientes. Mejora la extracción de datos en la página de Fasecolda con espera adicional para estabilización y optimiza el manejo de columnas en el manejador de plantillas.
</commit_message>
<xml_diff>
--- a/Bases Consolidados/PANTILLA CONFAMILIA N.xlsx
+++ b/Bases Consolidados/PANTILLA CONFAMILIA N.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\PROYECTOS\AGENCIA INFONDO\COTIZACIONES\MCP\Bases Consolidados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\PROYECTOS\AGENCIA INFONDO\COTIZACIONES\Bases Consolidados Nuevas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6088783E-453A-4DE8-A3B2-E4A77F4C3FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F2920C-A628-4ED0-8147-C712123FA81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Autos" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
   <si>
     <t>Fecha De Cotización</t>
   </si>
@@ -92,9 +92,6 @@
     <t>La presente cotización no constituye aceptación del riesgo por parte de LAS COMPAÑIAS ASEGURADORAS, hasta tanto la compañía se manifieste de manera expresa y en documento escrito. Este documento es una cotización de SEGUROS de su vehículo; en caso de expedirse la póliza las condiciones de esta oferta pueden variar. Los términos de la cotización están sujetos a las condiciones generales y particulares del seguro que se cotiza, así como cambios en la medida en que se modifique la legislación tributaria. Esta cotización tiene una vigencia de 15 días calendario posteriores a su elaboración.</t>
   </si>
   <si>
-    <t>LINEAS DE ASISTENCIA</t>
-  </si>
-  <si>
     <t>DEDUCIBLES</t>
   </si>
   <si>
@@ -122,20 +119,174 @@
     <t>CONDICIONES ECONOMICAS</t>
   </si>
   <si>
-    <t>Autos Parcial</t>
-  </si>
-  <si>
     <t>Solidaria</t>
   </si>
   <si>
     <t>COTIZACIÓN PÓLIZA COLECTIVA DE AUTOS CONFAMILIA</t>
+  </si>
+  <si>
+    <t>Responsabilidad civil extracontractual</t>
+  </si>
+  <si>
+    <t>Daños a bienes de terceros</t>
+  </si>
+  <si>
+    <t>Muerte o lesión a una persona</t>
+  </si>
+  <si>
+    <t>Muerte o lesiones a dos o más personas</t>
+  </si>
+  <si>
+    <t>Asistencia jurídica en proceso penal y civil</t>
+  </si>
+  <si>
+    <t>Pérdida total por daños</t>
+  </si>
+  <si>
+    <t>Pérdida parcial por daños</t>
+  </si>
+  <si>
+    <t>Pérdida total por hurto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terremoto </t>
+  </si>
+  <si>
+    <t>Amparo patrimonial</t>
+  </si>
+  <si>
+    <t>Gastos de transporte por pérdida total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehículo de reemplazo por pérdida total </t>
+  </si>
+  <si>
+    <t>Vehículo de reemplazo por pérdida parcial</t>
+  </si>
+  <si>
+    <t>Asistencia en viaje</t>
+  </si>
+  <si>
+    <t>Accidentes personales al conductor</t>
+  </si>
+  <si>
+    <t>Accidentes personales a ocupantes</t>
+  </si>
+  <si>
+    <t>Accidentes al viajero</t>
+  </si>
+  <si>
+    <t>Renta por hospitalización en viajes</t>
+  </si>
+  <si>
+    <t>Equipaje protegido</t>
+  </si>
+  <si>
+    <t>Hurto de documentos</t>
+  </si>
+  <si>
+    <t>Máximo $40.000.000</t>
+  </si>
+  <si>
+    <t>Incluido</t>
+  </si>
+  <si>
+    <t>$ 40.000 diarios hasta 
+por 30 días</t>
+  </si>
+  <si>
+    <t>Hasta por 20 días</t>
+  </si>
+  <si>
+    <t>Incluida</t>
+  </si>
+  <si>
+    <t>1.5 SMDLV hasta por 60 días</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hasta 8 dias</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hasta 5 dias</t>
+  </si>
+  <si>
+    <t>No cubierto</t>
+  </si>
+  <si>
+    <t>$ 30.000 diarios hasta 
+por 30 días</t>
+  </si>
+  <si>
+    <t>Hasta por 30 días</t>
+  </si>
+  <si>
+    <t>Hasta por 7 días</t>
+  </si>
+  <si>
+    <t>No incluye</t>
+  </si>
+  <si>
+    <t>Pérdida total por daños o hurto</t>
+  </si>
+  <si>
+    <t>Pérdida parcial por daños o hurto</t>
+  </si>
+  <si>
+    <t>1 SMLMV  para Automoviles,
+para Camperos y pick up 1 SMLMV</t>
+  </si>
+  <si>
+    <t>Si el arreglo cuesta menos de 2,5 smmlv deberás asumirlo, si es superior, SURA asume el valor.</t>
+  </si>
+  <si>
+    <t>1SMMLV</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Global Franquicia</t>
+  </si>
+  <si>
+    <t>SERVICIOS DE LA ASISTENCIA EN VIAJE</t>
+  </si>
+  <si>
+    <t>Revisión preventiva de viaje</t>
+  </si>
+  <si>
+    <t>Conductor elegido</t>
+  </si>
+  <si>
+    <t>Servicio de grúa</t>
+  </si>
+  <si>
+    <t>Carro taller</t>
+  </si>
+  <si>
+    <t>3 eventos por vigencia</t>
+  </si>
+  <si>
+    <t>12 eventos por vigencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 eventos por mes  </t>
+  </si>
+  <si>
+    <t>Hasta 50 SMDLV</t>
+  </si>
+  <si>
+    <t>10 eventos por vigencia</t>
+  </si>
+  <si>
+    <t>VALOR ASEGURADO AUTO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +336,19 @@
       <color rgb="FF002060"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -243,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -313,9 +477,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -326,9 +488,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -338,38 +498,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -385,22 +570,59 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,15 +637,50 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -436,115 +693,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>165287</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>157144</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1703294</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>567721</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4C7CB8F-7C0F-4666-8C82-3DC9BB48EC6D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="165287" y="157144"/>
-          <a:ext cx="1538007" cy="410577"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>280147</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1817699</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F7DE8A-601E-988D-CCA0-E9877D993E2F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8090647" y="78441"/>
-          <a:ext cx="1537552" cy="661148"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -844,166 +992,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8971C112-9AF6-42D6-81AB-E2C154B579CA}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="59.1" customHeight="1">
-      <c r="A1" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="A1" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="39"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="36"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="2"/>
@@ -1012,223 +1160,371 @@
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="10" t="s">
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="31"/>
+      <c r="B20" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="28"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="24"/>
-      <c r="B20" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="7"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="11"/>
+      <c r="B21" s="45">
+        <v>3040000000</v>
+      </c>
+      <c r="C21" s="45">
+        <v>3040000000</v>
+      </c>
+      <c r="D21" s="46">
+        <v>1000000000</v>
+      </c>
+      <c r="E21" s="46">
+        <v>2028000000</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="7"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="A22" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="7"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="A23" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="14">
+        <v>1000000000</v>
+      </c>
+      <c r="E23" s="14">
+        <v>2028000000</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="A24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="14">
+        <v>2000000000</v>
+      </c>
+      <c r="E24" s="14">
+        <v>4056000000</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
+      <c r="A25" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="7"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="A26" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="7"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="A27" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" ht="15.75">
-      <c r="A29" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
+      <c r="A28" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="7"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="A30" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75">
-      <c r="A32" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
+      <c r="A31" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30">
+      <c r="A32" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="13">
-        <v>45913</v>
-      </c>
-      <c r="C33" s="13">
-        <v>45913</v>
-      </c>
-      <c r="D33" s="13">
-        <v>45913</v>
-      </c>
-      <c r="E33" s="13">
-        <v>45913</v>
+      <c r="A33" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="13">
-        <v>45974</v>
-      </c>
-      <c r="C34" s="13">
-        <v>45971</v>
-      </c>
-      <c r="D34" s="13">
-        <v>45974</v>
-      </c>
-      <c r="E34" s="13">
-        <v>45974</v>
+      <c r="A34" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="15">
-        <v>61</v>
-      </c>
-      <c r="C35" s="15">
-        <v>58</v>
-      </c>
-      <c r="D35" s="15">
-        <v>61</v>
-      </c>
-      <c r="E35" s="15">
-        <v>61</v>
+      <c r="A35" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="16"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
+        <v>43</v>
+      </c>
+      <c r="B36" s="24">
+        <v>50000000</v>
+      </c>
+      <c r="C36" s="24">
+        <v>50000000</v>
+      </c>
+      <c r="D36" s="24">
+        <v>30000000</v>
+      </c>
+      <c r="E36" s="47" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
+      <c r="A37" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" s="14">
+        <v>35000000</v>
+      </c>
+      <c r="C37" s="14">
+        <v>35000000</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" s="47"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="A38" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-    </row>
-    <row r="40" spans="1:5" ht="44.25" customHeight="1">
-      <c r="A40" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
+      <c r="A39" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="A41" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1"/>
@@ -1238,32 +1534,64 @@
       <c r="E42" s="1"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="A43" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="31"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="A44" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44" s="16">
+        <v>0</v>
+      </c>
+      <c r="C44" s="16">
+        <v>0</v>
+      </c>
+      <c r="D44" s="16">
+        <v>0</v>
+      </c>
+      <c r="E44" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="A45" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B45" s="15">
+        <v>0</v>
+      </c>
+      <c r="C45" s="15">
+        <v>0</v>
+      </c>
+      <c r="D45" s="16">
+        <v>0</v>
+      </c>
+      <c r="E45" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="60">
+      <c r="A46" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1"/>
@@ -1272,41 +1600,247 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+    <row r="48" spans="1:5" ht="15.75">
+      <c r="A48" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="A49" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="1:5" ht="15.75">
+      <c r="A54" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="7">
+        <v>46296</v>
+      </c>
+      <c r="C56" s="7">
+        <v>46296</v>
+      </c>
+      <c r="D56" s="7">
+        <v>46068</v>
+      </c>
+      <c r="E56" s="7">
+        <v>46296</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B61" s="34"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+    </row>
+    <row r="62" spans="1:5" ht="44.25" customHeight="1">
+      <c r="A62" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="33"/>
+      <c r="C62" s="33"/>
+      <c r="D62" s="33"/>
+      <c r="E62" s="33"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A39:E39"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C16:E16"/>
+  <mergeCells count="40">
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="D21:D22"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A8:B8"/>
@@ -1323,26 +1857,44 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A54:E54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1472,6 +2024,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98AAA9BD-141C-449E-9A5F-E23FE59D0BF8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059BE399-E90A-4F5C-8B54-187AC91B948A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -1483,14 +2043,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="cb24288e-bf72-47ae-a461-19b0293297a2"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98AAA9BD-141C-449E-9A5F-E23FE59D0BF8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>